<commit_message>
couple of location lookup tables.
</commit_message>
<xml_diff>
--- a/data-raw/regionInformation/perennialCrops.xlsx
+++ b/data-raw/regionInformation/perennialCrops.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gcn/Documents/workspace/ISIMIPData/data-raw/regionInformation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B73EAC5F-74A0-CD42-A9FF-B5D2A5472448}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09EA3B45-235E-C146-B2DF-ACDC61574488}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5140" yWindow="21560" windowWidth="26440" windowHeight="15440" xr2:uid="{02F4FA97-6E90-D04F-8B97-AC9F3BC53EA0}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="27">
   <si>
     <t>region</t>
   </si>
@@ -50,12 +50,6 @@
     <t>longitude</t>
   </si>
   <si>
-    <t>Santiago</t>
-  </si>
-  <si>
-    <t>Chile</t>
-  </si>
-  <si>
     <t>Tasmania</t>
   </si>
   <si>
@@ -74,12 +68,6 @@
     <t>Pullman</t>
   </si>
   <si>
-    <t>New York</t>
-  </si>
-  <si>
-    <t>Ithaca</t>
-  </si>
-  <si>
     <t>Canberra</t>
   </si>
   <si>
@@ -105,9 +93,6 @@
   </si>
   <si>
     <t>USA</t>
-  </si>
-  <si>
-    <t>CHL</t>
   </si>
   <si>
     <t>AUS</t>
@@ -487,10 +472,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6B950FA-0A16-3042-B472-F300234D4FE0}">
-  <dimension ref="A1:K9"/>
+  <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -519,22 +504,22 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="G1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J1" t="s">
+        <v>15</v>
+      </c>
+      <c r="K1" t="s">
         <v>16</v>
-      </c>
-      <c r="H1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I1" t="s">
-        <v>18</v>
-      </c>
-      <c r="J1" t="s">
-        <v>19</v>
-      </c>
-      <c r="K1" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
@@ -545,263 +530,189 @@
         <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D2" s="1">
-        <v>-33.448889700000002</v>
+        <v>-42.834411500000002</v>
       </c>
       <c r="E2" s="1">
-        <v>-70.669265499999995</v>
+        <v>147.2330991</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="2">
-        <f t="shared" ref="G2:G8" si="0">ROUND(D2-B$9, 0)</f>
-        <v>-35</v>
+        <f>ROUND(D2-B$7, 0)</f>
+        <v>-45</v>
       </c>
       <c r="H2" s="2">
-        <f>ROUND(E2-$B$9, 0)</f>
-        <v>-73</v>
+        <f>ROUND(E2-$B$7, 0)</f>
+        <v>145</v>
       </c>
       <c r="I2" s="2">
-        <f t="shared" ref="I2:I7" si="1">ROUND(D2+B$9, 0)</f>
-        <v>-31</v>
+        <f>ROUND(D2+B$7, 0)</f>
+        <v>-41</v>
       </c>
       <c r="J2" s="2">
-        <f>ROUND(E2+B$9, 0)</f>
-        <v>-69</v>
+        <f>ROUND(E2+B$7, 0)</f>
+        <v>149</v>
       </c>
       <c r="K2" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D3" s="1">
-        <v>-42.834411500000002</v>
+        <v>46.731926199999997</v>
       </c>
       <c r="E3" s="1">
-        <v>147.2330991</v>
+        <v>-117.1564061</v>
       </c>
       <c r="F3" s="2"/>
       <c r="G3" s="2">
-        <f t="shared" si="0"/>
-        <v>-45</v>
+        <f>ROUND(D3-B$7, 0)</f>
+        <v>45</v>
       </c>
       <c r="H3" s="2">
-        <f t="shared" ref="H3:H8" si="2">ROUND(E3-$B$9, 0)</f>
-        <v>145</v>
+        <f>ROUND(E3-$B$7, 0)</f>
+        <v>-119</v>
       </c>
       <c r="I3" s="2">
-        <f t="shared" si="1"/>
-        <v>-41</v>
+        <f>ROUND(D3+B$7, 0)</f>
+        <v>49</v>
       </c>
       <c r="J3" s="2">
-        <f t="shared" ref="J3:J8" si="3">ROUND(E3+B$9, 0)</f>
-        <v>149</v>
+        <f>ROUND(E3+B$7, 0)</f>
+        <v>-115</v>
       </c>
       <c r="K3" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" t="s">
         <v>11</v>
       </c>
-      <c r="C4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" s="1">
-        <v>46.731926199999997</v>
+      <c r="D4" s="3">
+        <v>-35.3138194</v>
       </c>
       <c r="E4" s="1">
-        <v>-117.1564061</v>
+        <v>149.05957190000001</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="2">
-        <f t="shared" si="0"/>
-        <v>45</v>
+        <f>ROUND(D4-B$7, 0)</f>
+        <v>-37</v>
       </c>
       <c r="H4" s="2">
-        <f t="shared" si="2"/>
-        <v>-119</v>
+        <f>ROUND(E4-$B$7, 0)</f>
+        <v>147</v>
       </c>
       <c r="I4" s="2">
-        <f t="shared" si="1"/>
-        <v>49</v>
+        <f>ROUND(D4+B$7, 0)</f>
+        <v>-33</v>
       </c>
       <c r="J4" s="2">
-        <f t="shared" si="3"/>
-        <v>-115</v>
+        <f>ROUND(E4+B$7, 0)</f>
+        <v>151</v>
       </c>
       <c r="K4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="C5" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="D5" s="1">
-        <v>42.453453099999997</v>
+        <v>55.941284500000002</v>
       </c>
       <c r="E5" s="1">
-        <v>-76.4756967</v>
-      </c>
-      <c r="F5" s="2"/>
+        <v>-3.2755491999999999</v>
+      </c>
       <c r="G5" s="2">
-        <f t="shared" si="0"/>
-        <v>40</v>
+        <f>ROUND(D5-B$7, 0)</f>
+        <v>54</v>
       </c>
       <c r="H5" s="2">
-        <f t="shared" si="2"/>
-        <v>-78</v>
+        <f>ROUND(E5-$B$7, 0)</f>
+        <v>-5</v>
       </c>
       <c r="I5" s="2">
-        <f t="shared" si="1"/>
-        <v>44</v>
+        <f>ROUND(D5+B$7, 0)</f>
+        <v>58</v>
       </c>
       <c r="J5" s="2">
-        <f t="shared" si="3"/>
-        <v>-74</v>
+        <f>ROUND(E5+B$7, 0)</f>
+        <v>-1</v>
       </c>
       <c r="K5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="B6" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>15</v>
-      </c>
-      <c r="D6" s="3">
-        <v>-35.3138194</v>
+        <v>25</v>
+      </c>
+      <c r="D6" s="1">
+        <v>40.029420199999997</v>
       </c>
       <c r="E6" s="1">
-        <v>149.05957190000001</v>
-      </c>
-      <c r="F6" s="2"/>
+        <v>-105.3101887</v>
+      </c>
+      <c r="F6" t="s">
+        <v>26</v>
+      </c>
       <c r="G6" s="2">
-        <f t="shared" si="0"/>
-        <v>-37</v>
+        <f t="shared" ref="G6" si="0">ROUND(D6-B$7, 0)</f>
+        <v>38</v>
       </c>
       <c r="H6" s="2">
-        <f t="shared" si="2"/>
-        <v>147</v>
+        <f t="shared" ref="H6" si="1">ROUND(E6-$B$7, 0)</f>
+        <v>-107</v>
       </c>
       <c r="I6" s="2">
-        <f t="shared" si="1"/>
-        <v>-33</v>
+        <f t="shared" ref="I6" si="2">ROUND(D6+B$7, 0)</f>
+        <v>42</v>
       </c>
       <c r="J6" s="2">
-        <f t="shared" si="3"/>
-        <v>151</v>
+        <f t="shared" ref="J6" si="3">ROUND(E6+B$7, 0)</f>
+        <v>-103</v>
       </c>
       <c r="K6" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>26</v>
-      </c>
-      <c r="B7" t="s">
-        <v>28</v>
-      </c>
-      <c r="C7" t="s">
-        <v>26</v>
-      </c>
-      <c r="D7" s="1">
-        <v>55.941284500000002</v>
-      </c>
-      <c r="E7" s="1">
-        <v>-3.2755491999999999</v>
-      </c>
-      <c r="G7" s="2">
-        <f t="shared" si="0"/>
-        <v>54</v>
-      </c>
-      <c r="H7" s="2">
-        <f t="shared" si="2"/>
-        <v>-5</v>
-      </c>
-      <c r="I7" s="2">
-        <f t="shared" si="1"/>
-        <v>58</v>
-      </c>
-      <c r="J7" s="2">
-        <f t="shared" si="3"/>
-        <v>-1</v>
-      </c>
-      <c r="K7" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>29</v>
-      </c>
-      <c r="B8" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" t="s">
-        <v>30</v>
-      </c>
-      <c r="D8" s="1">
-        <v>40.029420199999997</v>
-      </c>
-      <c r="E8" s="1">
-        <v>-105.3101887</v>
-      </c>
-      <c r="F8" t="s">
-        <v>31</v>
-      </c>
-      <c r="G8" s="2">
-        <f t="shared" ref="G8" si="4">ROUND(D8-B$9, 0)</f>
-        <v>38</v>
-      </c>
-      <c r="H8" s="2">
-        <f t="shared" ref="H8" si="5">ROUND(E8-$B$9, 0)</f>
-        <v>-107</v>
-      </c>
-      <c r="I8" s="2">
-        <f t="shared" ref="I8" si="6">ROUND(D8+B$9, 0)</f>
-        <v>42</v>
-      </c>
-      <c r="J8" s="2">
-        <f t="shared" ref="J8" si="7">ROUND(E8+B$9, 0)</f>
-        <v>-103</v>
-      </c>
-      <c r="K8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>21</v>
-      </c>
-      <c r="B9">
+        <v>17</v>
+      </c>
+      <c r="B7">
         <v>2</v>
       </c>
     </row>

</xml_diff>